<commit_message>
10.8.20 update with changes to time axis
</commit_message>
<xml_diff>
--- a/data/fiona_diaper.xlsx
+++ b/data/fiona_diaper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Fiona/fiona_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB01C2C-4266-7245-871D-E61FADAB1379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B043F-81A5-B24D-86D9-611AFC6520FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{B859BB0C-59A7-8246-A5B9-DC632F951B06}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -403,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7482C379-60CB-834D-835A-65354080E5E1}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A216" sqref="A216"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -571,7 +571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -591,7 +591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -611,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -631,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -731,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -751,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -771,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -791,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -871,7 +871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -891,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -911,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -931,7 +931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -951,7 +951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -971,7 +971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>211</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
@@ -4708,6 +4708,526 @@
         <v>0</v>
       </c>
       <c r="F215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" s="1">
+        <v>44087</v>
+      </c>
+      <c r="C216">
+        <v>5</v>
+      </c>
+      <c r="D216">
+        <v>4</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" s="1">
+        <v>44088</v>
+      </c>
+      <c r="C217">
+        <v>5</v>
+      </c>
+      <c r="D217">
+        <v>4</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" s="1">
+        <v>44089</v>
+      </c>
+      <c r="C218">
+        <v>5</v>
+      </c>
+      <c r="D218">
+        <v>5</v>
+      </c>
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" s="1">
+        <v>44090</v>
+      </c>
+      <c r="C219">
+        <v>5</v>
+      </c>
+      <c r="D219">
+        <v>5</v>
+      </c>
+      <c r="E219">
+        <v>0</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" s="1">
+        <v>44091</v>
+      </c>
+      <c r="C220">
+        <v>6</v>
+      </c>
+      <c r="D220">
+        <v>4</v>
+      </c>
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221" s="1">
+        <v>44092</v>
+      </c>
+      <c r="C221">
+        <v>5</v>
+      </c>
+      <c r="D221">
+        <v>5</v>
+      </c>
+      <c r="E221">
+        <v>0</v>
+      </c>
+      <c r="F221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222" s="1">
+        <v>44093</v>
+      </c>
+      <c r="C222">
+        <v>5</v>
+      </c>
+      <c r="D222">
+        <v>5</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223" s="1">
+        <v>44094</v>
+      </c>
+      <c r="C223">
+        <v>5</v>
+      </c>
+      <c r="D223">
+        <v>4</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224" s="1">
+        <v>44095</v>
+      </c>
+      <c r="C224">
+        <v>5</v>
+      </c>
+      <c r="D224">
+        <v>5</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225" s="1">
+        <v>44096</v>
+      </c>
+      <c r="C225">
+        <v>6</v>
+      </c>
+      <c r="D225">
+        <v>6</v>
+      </c>
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226" s="1">
+        <v>44097</v>
+      </c>
+      <c r="C226">
+        <v>6</v>
+      </c>
+      <c r="D226">
+        <v>6</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C227">
+        <v>6</v>
+      </c>
+      <c r="D227">
+        <v>6</v>
+      </c>
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228" s="1">
+        <v>44099</v>
+      </c>
+      <c r="C228">
+        <v>5</v>
+      </c>
+      <c r="D228">
+        <v>5</v>
+      </c>
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229" s="1">
+        <v>44100</v>
+      </c>
+      <c r="C229">
+        <v>5</v>
+      </c>
+      <c r="D229">
+        <v>4</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230" s="1">
+        <v>44101</v>
+      </c>
+      <c r="C230">
+        <v>6</v>
+      </c>
+      <c r="D230">
+        <v>5</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231" s="1">
+        <v>44102</v>
+      </c>
+      <c r="C231">
+        <v>5</v>
+      </c>
+      <c r="D231">
+        <v>5</v>
+      </c>
+      <c r="E231">
+        <v>0</v>
+      </c>
+      <c r="F231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232" s="1">
+        <v>44103</v>
+      </c>
+      <c r="C232">
+        <v>5</v>
+      </c>
+      <c r="D232">
+        <v>5</v>
+      </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233" s="1">
+        <v>44104</v>
+      </c>
+      <c r="C233">
+        <v>6</v>
+      </c>
+      <c r="D233">
+        <v>5</v>
+      </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
+      <c r="F233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" s="1">
+        <v>44105</v>
+      </c>
+      <c r="C234">
+        <v>5</v>
+      </c>
+      <c r="D234">
+        <v>5</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" s="1">
+        <v>44106</v>
+      </c>
+      <c r="C235">
+        <v>5</v>
+      </c>
+      <c r="D235">
+        <v>5</v>
+      </c>
+      <c r="E235">
+        <v>0</v>
+      </c>
+      <c r="F235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" s="1">
+        <v>44107</v>
+      </c>
+      <c r="C236">
+        <v>5</v>
+      </c>
+      <c r="D236">
+        <v>4</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+      <c r="F236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" s="1">
+        <v>44108</v>
+      </c>
+      <c r="C237">
+        <v>6</v>
+      </c>
+      <c r="D237">
+        <v>5</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+      <c r="F237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" s="1">
+        <v>44109</v>
+      </c>
+      <c r="C238">
+        <v>4</v>
+      </c>
+      <c r="D238">
+        <v>4</v>
+      </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" s="1">
+        <v>44110</v>
+      </c>
+      <c r="C239">
+        <v>7</v>
+      </c>
+      <c r="D239">
+        <v>7</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" s="1">
+        <v>44111</v>
+      </c>
+      <c r="C240">
+        <v>6</v>
+      </c>
+      <c r="D240">
+        <v>5</v>
+      </c>
+      <c r="E240">
+        <v>0</v>
+      </c>
+      <c r="F240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" s="1">
+        <v>44112</v>
+      </c>
+      <c r="C241">
+        <v>5</v>
+      </c>
+      <c r="D241">
+        <v>5</v>
+      </c>
+      <c r="E241">
+        <v>0</v>
+      </c>
+      <c r="F241">
         <v>0</v>
       </c>
     </row>

</xml_diff>